<commit_message>
update "generate_output" function argument to include "parm"
</commit_message>
<xml_diff>
--- a/examples/SimpleFe/model_parsing_diagnostics.SimpleFe.xlsx
+++ b/examples/SimpleFe/model_parsing_diagnostics.SimpleFe.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="183">
   <si>
     <t>label</t>
   </si>
@@ -580,9 +580,6 @@
   </si>
   <si>
     <t>kFeOOHH2S</t>
-  </si>
-  <si>
-    <t>kFeSpre</t>
   </si>
 </sst>
 </file>
@@ -2963,7 +2960,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -3090,17 +3087,6 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>183</v>
-      </c>
-      <c r="B12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>